<commit_message>
SQL Database y CartaGantt
SQL tablas iniciales
</commit_message>
<xml_diff>
--- a/Fase 1/Evidencias Grupales/CartaGantt.xlsx
+++ b/Fase 1/Evidencias Grupales/CartaGantt.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2542A04C-B07C-4AE7-BF98-E21C0EDD1FA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D452A3D-CA26-4224-B003-1E9945781815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="calendarioproyecto" sheetId="11" r:id="rId1"/>
@@ -1378,6 +1378,162 @@
     <xf numFmtId="172" fontId="29" fillId="42" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="44" borderId="2" xfId="12" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="44" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="44" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="9" fillId="44" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="30" fillId="10" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="45" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="45" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="45" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="45" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="5" fillId="45" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="46" borderId="2" xfId="12" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="46" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="46" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="9" fillId="46" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="47" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="47" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="47" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="47" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="5" fillId="47" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="48" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="48" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="48" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="48" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="5" fillId="48" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="49" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="49" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="49" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="49" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="5" fillId="49" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="50" borderId="2" xfId="12" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="50" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="50" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="9" fillId="50" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="51" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="51" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="51" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="51" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="5" fillId="51" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="52" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="52" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="52" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="52" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="5" fillId="52" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="53" borderId="2" xfId="12" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="53" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="53" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="9" fillId="53" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="54" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="54" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="54" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="54" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="5" fillId="54" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="171" fontId="15" fillId="42" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1387,9 +1543,6 @@
     <xf numFmtId="171" fontId="15" fillId="42" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="170" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -1397,160 +1550,7 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="44" borderId="2" xfId="12" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="44" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="44" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="9" fillId="44" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="30" fillId="10" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="45" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="45" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="45" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="45" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="5" fillId="45" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="46" borderId="2" xfId="12" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="46" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="46" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="9" fillId="46" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="47" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="47" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="47" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="47" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="5" fillId="47" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="48" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="48" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="48" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="48" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="5" fillId="48" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="49" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="49" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="49" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="49" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="5" fillId="49" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="50" borderId="2" xfId="12" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="50" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="50" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="9" fillId="50" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="51" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="51" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="51" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="51" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="5" fillId="51" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="52" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="52" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="52" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="52" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="5" fillId="52" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="53" borderId="2" xfId="12" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="53" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="53" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="9" fillId="53" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="54" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="54" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="54" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="54" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="5" fillId="54" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="9" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1611,7 +1611,7 @@
     <cellStyle name="Total" xfId="29" builtinId="25" customBuiltin="1"/>
     <cellStyle name="zTextoOculto" xfId="3" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="14">
     <dxf>
       <fill>
         <patternFill>
@@ -1622,13 +1622,6 @@
         <left/>
         <right/>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <border>
@@ -1645,6 +1638,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00B0F0"/>
         </patternFill>
       </fill>
@@ -1652,13 +1652,6 @@
         <left/>
         <right/>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <border>
@@ -1768,15 +1761,15 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="ListaTareasPendientes" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="14"/>
-      <tableStyleElement type="headerRow" dxfId="13"/>
-      <tableStyleElement type="totalRow" dxfId="12"/>
-      <tableStyleElement type="firstColumn" dxfId="11"/>
-      <tableStyleElement type="lastColumn" dxfId="10"/>
-      <tableStyleElement type="firstRowStripe" dxfId="9"/>
-      <tableStyleElement type="secondRowStripe" dxfId="8"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="7"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="6"/>
+      <tableStyleElement type="wholeTable" dxfId="13"/>
+      <tableStyleElement type="headerRow" dxfId="12"/>
+      <tableStyleElement type="totalRow" dxfId="11"/>
+      <tableStyleElement type="firstColumn" dxfId="10"/>
+      <tableStyleElement type="lastColumn" dxfId="9"/>
+      <tableStyleElement type="firstRowStripe" dxfId="8"/>
+      <tableStyleElement type="secondRowStripe" dxfId="7"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="6"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="5"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -2271,26 +2264,26 @@
   </sheetPr>
   <dimension ref="A1:CG51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="69" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="32" customWidth="1"/>
-    <col min="2" max="2" width="54.85546875" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" customWidth="1"/>
-    <col min="7" max="7" width="2.7109375" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" hidden="1" customWidth="1"/>
-    <col min="9" max="85" width="2.5703125" customWidth="1"/>
-    <col min="90" max="91" width="10.28515625"/>
+    <col min="1" max="1" width="2.73046875" style="32" customWidth="1"/>
+    <col min="2" max="2" width="54.86328125" customWidth="1"/>
+    <col min="3" max="3" width="23.86328125" customWidth="1"/>
+    <col min="4" max="4" width="10.73046875" customWidth="1"/>
+    <col min="5" max="5" width="10.3984375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.3984375" customWidth="1"/>
+    <col min="7" max="7" width="2.73046875" customWidth="1"/>
+    <col min="8" max="8" width="6.1328125" hidden="1" customWidth="1"/>
+    <col min="9" max="85" width="2.59765625" customWidth="1"/>
+    <col min="90" max="91" width="10.265625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:85" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:85" ht="30" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
@@ -2306,7 +2299,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:85" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:85" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
@@ -2315,155 +2308,155 @@
       </c>
       <c r="I2" s="35"/>
     </row>
-    <row r="3" spans="1:85" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:85" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="32" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="81" t="s">
+      <c r="C3" s="132" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="82"/>
-      <c r="E3" s="80">
+      <c r="D3" s="133"/>
+      <c r="E3" s="135">
         <f ca="1">TODAY()</f>
-        <v>45926</v>
-      </c>
-      <c r="F3" s="80"/>
+        <v>45927</v>
+      </c>
+      <c r="F3" s="135"/>
     </row>
-    <row r="4" spans="1:85" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:85" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="81" t="s">
+      <c r="C4" s="132" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="82"/>
+      <c r="D4" s="133"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="77">
+      <c r="I4" s="129">
         <f ca="1">I5</f>
         <v>45922</v>
       </c>
-      <c r="J4" s="78"/>
-      <c r="K4" s="78"/>
-      <c r="L4" s="78"/>
-      <c r="M4" s="78"/>
-      <c r="N4" s="78"/>
-      <c r="O4" s="79"/>
-      <c r="P4" s="77">
+      <c r="J4" s="130"/>
+      <c r="K4" s="130"/>
+      <c r="L4" s="130"/>
+      <c r="M4" s="130"/>
+      <c r="N4" s="130"/>
+      <c r="O4" s="131"/>
+      <c r="P4" s="129">
         <f ca="1">P5</f>
         <v>45929</v>
       </c>
-      <c r="Q4" s="78"/>
-      <c r="R4" s="78"/>
-      <c r="S4" s="78"/>
-      <c r="T4" s="78"/>
-      <c r="U4" s="78"/>
-      <c r="V4" s="79"/>
-      <c r="W4" s="77">
+      <c r="Q4" s="130"/>
+      <c r="R4" s="130"/>
+      <c r="S4" s="130"/>
+      <c r="T4" s="130"/>
+      <c r="U4" s="130"/>
+      <c r="V4" s="131"/>
+      <c r="W4" s="129">
         <f ca="1">W5</f>
         <v>45936</v>
       </c>
-      <c r="X4" s="78"/>
-      <c r="Y4" s="78"/>
-      <c r="Z4" s="78"/>
-      <c r="AA4" s="78"/>
-      <c r="AB4" s="78"/>
-      <c r="AC4" s="79"/>
-      <c r="AD4" s="77">
+      <c r="X4" s="130"/>
+      <c r="Y4" s="130"/>
+      <c r="Z4" s="130"/>
+      <c r="AA4" s="130"/>
+      <c r="AB4" s="130"/>
+      <c r="AC4" s="131"/>
+      <c r="AD4" s="129">
         <f ca="1">AD5</f>
         <v>45943</v>
       </c>
-      <c r="AE4" s="78"/>
-      <c r="AF4" s="78"/>
-      <c r="AG4" s="78"/>
-      <c r="AH4" s="78"/>
-      <c r="AI4" s="78"/>
-      <c r="AJ4" s="79"/>
-      <c r="AK4" s="77">
+      <c r="AE4" s="130"/>
+      <c r="AF4" s="130"/>
+      <c r="AG4" s="130"/>
+      <c r="AH4" s="130"/>
+      <c r="AI4" s="130"/>
+      <c r="AJ4" s="131"/>
+      <c r="AK4" s="129">
         <f ca="1">AK5</f>
         <v>45950</v>
       </c>
-      <c r="AL4" s="78"/>
-      <c r="AM4" s="78"/>
-      <c r="AN4" s="78"/>
-      <c r="AO4" s="78"/>
-      <c r="AP4" s="78"/>
-      <c r="AQ4" s="79"/>
-      <c r="AR4" s="77">
+      <c r="AL4" s="130"/>
+      <c r="AM4" s="130"/>
+      <c r="AN4" s="130"/>
+      <c r="AO4" s="130"/>
+      <c r="AP4" s="130"/>
+      <c r="AQ4" s="131"/>
+      <c r="AR4" s="129">
         <f ca="1">AR5</f>
         <v>45957</v>
       </c>
-      <c r="AS4" s="78"/>
-      <c r="AT4" s="78"/>
-      <c r="AU4" s="78"/>
-      <c r="AV4" s="78"/>
-      <c r="AW4" s="78"/>
-      <c r="AX4" s="79"/>
-      <c r="AY4" s="77">
+      <c r="AS4" s="130"/>
+      <c r="AT4" s="130"/>
+      <c r="AU4" s="130"/>
+      <c r="AV4" s="130"/>
+      <c r="AW4" s="130"/>
+      <c r="AX4" s="131"/>
+      <c r="AY4" s="129">
         <f ca="1">AY5</f>
         <v>45964</v>
       </c>
-      <c r="AZ4" s="78"/>
-      <c r="BA4" s="78"/>
-      <c r="BB4" s="78"/>
-      <c r="BC4" s="78"/>
-      <c r="BD4" s="78"/>
-      <c r="BE4" s="79"/>
-      <c r="BF4" s="77">
+      <c r="AZ4" s="130"/>
+      <c r="BA4" s="130"/>
+      <c r="BB4" s="130"/>
+      <c r="BC4" s="130"/>
+      <c r="BD4" s="130"/>
+      <c r="BE4" s="131"/>
+      <c r="BF4" s="129">
         <f ca="1">BF5</f>
         <v>45971</v>
       </c>
-      <c r="BG4" s="78"/>
-      <c r="BH4" s="78"/>
-      <c r="BI4" s="78"/>
-      <c r="BJ4" s="78"/>
-      <c r="BK4" s="78"/>
-      <c r="BL4" s="79"/>
-      <c r="BM4" s="77">
+      <c r="BG4" s="130"/>
+      <c r="BH4" s="130"/>
+      <c r="BI4" s="130"/>
+      <c r="BJ4" s="130"/>
+      <c r="BK4" s="130"/>
+      <c r="BL4" s="131"/>
+      <c r="BM4" s="129">
         <f ca="1">BM5</f>
         <v>45978</v>
       </c>
-      <c r="BN4" s="78"/>
-      <c r="BO4" s="78"/>
-      <c r="BP4" s="78"/>
-      <c r="BQ4" s="78"/>
-      <c r="BR4" s="78"/>
-      <c r="BS4" s="79"/>
-      <c r="BT4" s="77">
+      <c r="BN4" s="130"/>
+      <c r="BO4" s="130"/>
+      <c r="BP4" s="130"/>
+      <c r="BQ4" s="130"/>
+      <c r="BR4" s="130"/>
+      <c r="BS4" s="131"/>
+      <c r="BT4" s="129">
         <f ca="1">BT5</f>
         <v>45985</v>
       </c>
-      <c r="BU4" s="78"/>
-      <c r="BV4" s="78"/>
-      <c r="BW4" s="78"/>
-      <c r="BX4" s="78"/>
-      <c r="BY4" s="78"/>
-      <c r="BZ4" s="79"/>
-      <c r="CA4" s="77">
+      <c r="BU4" s="130"/>
+      <c r="BV4" s="130"/>
+      <c r="BW4" s="130"/>
+      <c r="BX4" s="130"/>
+      <c r="BY4" s="130"/>
+      <c r="BZ4" s="131"/>
+      <c r="CA4" s="129">
         <f ca="1">CA5</f>
         <v>45992</v>
       </c>
-      <c r="CB4" s="78"/>
-      <c r="CC4" s="78"/>
-      <c r="CD4" s="78"/>
-      <c r="CE4" s="78"/>
-      <c r="CF4" s="78"/>
-      <c r="CG4" s="79"/>
+      <c r="CB4" s="130"/>
+      <c r="CC4" s="130"/>
+      <c r="CD4" s="130"/>
+      <c r="CE4" s="130"/>
+      <c r="CF4" s="130"/>
+      <c r="CG4" s="131"/>
     </row>
-    <row r="5" spans="1:85" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:85" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="83"/>
-      <c r="C5" s="83"/>
-      <c r="D5" s="83"/>
-      <c r="E5" s="83"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
+      <c r="B5" s="134"/>
+      <c r="C5" s="134"/>
+      <c r="D5" s="134"/>
+      <c r="E5" s="134"/>
+      <c r="F5" s="134"/>
+      <c r="G5" s="134"/>
       <c r="I5" s="74">
         <f ca="1">InicioDelProyecto-WEEKDAY(InicioDelProyecto,1)+2+7*(SemanaParaMostrar-1)</f>
         <v>45922</v>
@@ -2773,7 +2766,7 @@
         <v>45998</v>
       </c>
     </row>
-    <row r="6" spans="1:85" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:85" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="33" t="s">
         <v>5</v>
       </c>
@@ -3105,7 +3098,7 @@
         <v>d</v>
       </c>
     </row>
-    <row r="7" spans="1:85" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:85" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="32" t="s">
         <v>6</v>
       </c>
@@ -3193,7 +3186,7 @@
       <c r="CF7" s="28"/>
       <c r="CG7" s="28"/>
     </row>
-    <row r="8" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="33" t="s">
         <v>7</v>
       </c>
@@ -3287,7 +3280,7 @@
       <c r="CF8" s="28"/>
       <c r="CG8" s="28"/>
     </row>
-    <row r="9" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="33" t="s">
         <v>8</v>
       </c>
@@ -3298,7 +3291,7 @@
         <v>19</v>
       </c>
       <c r="D9" s="14">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="E9" s="56">
         <v>45929</v>
@@ -3389,7 +3382,7 @@
       <c r="CF9" s="28"/>
       <c r="CG9" s="28"/>
     </row>
-    <row r="10" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A10" s="33" t="s">
         <v>9</v>
       </c>
@@ -3398,7 +3391,7 @@
       </c>
       <c r="C10" s="41"/>
       <c r="D10" s="14">
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="E10" s="56">
         <v>45932</v>
@@ -3490,7 +3483,7 @@
       <c r="CF10" s="28"/>
       <c r="CG10" s="28"/>
     </row>
-    <row r="11" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="33" t="s">
         <v>10</v>
       </c>
@@ -3584,14 +3577,14 @@
       <c r="CF11" s="28"/>
       <c r="CG11" s="28"/>
     </row>
-    <row r="12" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" s="33"/>
       <c r="B12" s="50" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="43"/>
       <c r="D12" s="17">
-        <v>0</v>
+        <v>0.88</v>
       </c>
       <c r="E12" s="59">
         <v>45934</v>
@@ -3682,7 +3675,7 @@
       <c r="CF12" s="28"/>
       <c r="CG12" s="28"/>
     </row>
-    <row r="13" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="33"/>
       <c r="B13" s="50" t="s">
         <v>32</v>
@@ -3777,7 +3770,7 @@
       <c r="CF13" s="28"/>
       <c r="CG13" s="28"/>
     </row>
-    <row r="14" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="32"/>
       <c r="B14" s="50" t="s">
         <v>33</v>
@@ -3875,7 +3868,7 @@
       <c r="CF14" s="28"/>
       <c r="CG14" s="28"/>
     </row>
-    <row r="15" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" s="32" t="s">
         <v>11</v>
       </c>
@@ -3969,7 +3962,7 @@
       <c r="CF15" s="28"/>
       <c r="CG15" s="28"/>
     </row>
-    <row r="16" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="32"/>
       <c r="B16" s="51" t="s">
         <v>35</v>
@@ -4067,7 +4060,7 @@
       <c r="CF16" s="28"/>
       <c r="CG16" s="28"/>
     </row>
-    <row r="17" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="32"/>
       <c r="B17" s="51" t="s">
         <v>36</v>
@@ -4166,7 +4159,7 @@
       <c r="CF17" s="28"/>
       <c r="CG17" s="28"/>
     </row>
-    <row r="18" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A18" s="32"/>
       <c r="B18" s="51" t="s">
         <v>37</v>
@@ -4264,13 +4257,13 @@
       <c r="CF18" s="28"/>
       <c r="CG18" s="28"/>
     </row>
-    <row r="19" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A19" s="32"/>
       <c r="B19" s="51" t="s">
         <v>38</v>
       </c>
       <c r="C19" s="45"/>
-      <c r="D19" s="88"/>
+      <c r="D19" s="81"/>
       <c r="E19" s="62"/>
       <c r="F19" s="62"/>
       <c r="G19" s="11"/>
@@ -4356,7 +4349,7 @@
       <c r="CF19" s="28"/>
       <c r="CG19" s="28"/>
     </row>
-    <row r="20" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A20" s="32" t="s">
         <v>11</v>
       </c>
@@ -4450,7 +4443,7 @@
       <c r="CF20" s="28"/>
       <c r="CG20" s="28"/>
     </row>
-    <row r="21" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A21" s="32"/>
       <c r="B21" s="52" t="s">
         <v>40</v>
@@ -4548,7 +4541,7 @@
       <c r="CF21" s="28"/>
       <c r="CG21" s="28"/>
     </row>
-    <row r="22" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A22" s="32"/>
       <c r="B22" s="52" t="s">
         <v>41</v>
@@ -4646,7 +4639,7 @@
       <c r="CF22" s="28"/>
       <c r="CG22" s="28"/>
     </row>
-    <row r="23" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A23" s="32"/>
       <c r="B23" s="52" t="s">
         <v>42</v>
@@ -4742,7 +4735,7 @@
       <c r="CF23" s="28"/>
       <c r="CG23" s="28"/>
     </row>
-    <row r="24" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A24" s="32"/>
       <c r="B24" s="52" t="s">
         <v>43</v>
@@ -4838,15 +4831,15 @@
       <c r="CF24" s="28"/>
       <c r="CG24" s="28"/>
     </row>
-    <row r="25" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A25" s="32"/>
-      <c r="B25" s="89" t="s">
+      <c r="B25" s="82" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="90"/>
-      <c r="D25" s="91"/>
-      <c r="E25" s="92"/>
-      <c r="F25" s="93"/>
+      <c r="C25" s="83"/>
+      <c r="D25" s="84"/>
+      <c r="E25" s="85"/>
+      <c r="F25" s="86"/>
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
       <c r="I25" s="28"/>
@@ -4927,19 +4920,19 @@
       <c r="CF25" s="28"/>
       <c r="CG25" s="28"/>
     </row>
-    <row r="26" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A26" s="32"/>
-      <c r="B26" s="84" t="s">
+      <c r="B26" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="85"/>
-      <c r="D26" s="86">
+      <c r="C26" s="78"/>
+      <c r="D26" s="79">
         <v>0</v>
       </c>
-      <c r="E26" s="87">
+      <c r="E26" s="80">
         <v>45962</v>
       </c>
-      <c r="F26" s="87">
+      <c r="F26" s="80">
         <v>45967</v>
       </c>
       <c r="G26" s="11"/>
@@ -5022,19 +5015,19 @@
       <c r="CF26" s="28"/>
       <c r="CG26" s="28"/>
     </row>
-    <row r="27" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A27" s="32"/>
-      <c r="B27" s="84" t="s">
+      <c r="B27" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="85"/>
-      <c r="D27" s="86">
+      <c r="C27" s="78"/>
+      <c r="D27" s="79">
         <v>0</v>
       </c>
-      <c r="E27" s="87">
+      <c r="E27" s="80">
         <v>45968</v>
       </c>
-      <c r="F27" s="87">
+      <c r="F27" s="80">
         <v>45971</v>
       </c>
       <c r="G27" s="11"/>
@@ -5117,17 +5110,17 @@
       <c r="CF27" s="28"/>
       <c r="CG27" s="28"/>
     </row>
-    <row r="28" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A28" s="32"/>
-      <c r="B28" s="84" t="s">
+      <c r="B28" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="85"/>
-      <c r="D28" s="86"/>
-      <c r="E28" s="87" t="s">
+      <c r="C28" s="78"/>
+      <c r="D28" s="79"/>
+      <c r="E28" s="80" t="s">
         <v>22</v>
       </c>
-      <c r="F28" s="87" t="s">
+      <c r="F28" s="80" t="s">
         <v>22</v>
       </c>
       <c r="G28" s="11"/>
@@ -5210,15 +5203,15 @@
       <c r="CF28" s="28"/>
       <c r="CG28" s="28"/>
     </row>
-    <row r="29" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A29" s="32"/>
-      <c r="B29" s="98" t="s">
+      <c r="B29" s="91" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="99"/>
-      <c r="D29" s="100"/>
-      <c r="E29" s="101"/>
-      <c r="F29" s="102"/>
+      <c r="C29" s="92"/>
+      <c r="D29" s="93"/>
+      <c r="E29" s="94"/>
+      <c r="F29" s="95"/>
       <c r="G29" s="11"/>
       <c r="H29" s="11"/>
       <c r="I29" s="28"/>
@@ -5299,19 +5292,19 @@
       <c r="CF29" s="28"/>
       <c r="CG29" s="28"/>
     </row>
-    <row r="30" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A30" s="32"/>
-      <c r="B30" s="94" t="s">
+      <c r="B30" s="87" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="95"/>
-      <c r="D30" s="96">
+      <c r="C30" s="88"/>
+      <c r="D30" s="89">
         <v>0</v>
       </c>
-      <c r="E30" s="97">
+      <c r="E30" s="90">
         <v>45972</v>
       </c>
-      <c r="F30" s="97">
+      <c r="F30" s="90">
         <v>45975</v>
       </c>
       <c r="G30" s="11"/>
@@ -5394,17 +5387,17 @@
       <c r="CF30" s="28"/>
       <c r="CG30" s="28"/>
     </row>
-    <row r="31" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A31" s="32"/>
-      <c r="B31" s="94" t="s">
+      <c r="B31" s="87" t="s">
         <v>50</v>
       </c>
-      <c r="C31" s="95"/>
-      <c r="D31" s="96"/>
-      <c r="E31" s="97" t="s">
+      <c r="C31" s="88"/>
+      <c r="D31" s="89"/>
+      <c r="E31" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="F31" s="97" t="s">
+      <c r="F31" s="90" t="s">
         <v>22</v>
       </c>
       <c r="G31" s="11"/>
@@ -5487,15 +5480,15 @@
       <c r="CF31" s="28"/>
       <c r="CG31" s="28"/>
     </row>
-    <row r="32" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A32" s="32"/>
-      <c r="B32" s="108" t="s">
+      <c r="B32" s="101" t="s">
         <v>51</v>
       </c>
-      <c r="C32" s="109"/>
-      <c r="D32" s="110"/>
-      <c r="E32" s="111"/>
-      <c r="F32" s="112"/>
+      <c r="C32" s="102"/>
+      <c r="D32" s="103"/>
+      <c r="E32" s="104"/>
+      <c r="F32" s="105"/>
       <c r="G32" s="11"/>
       <c r="H32" s="11"/>
       <c r="I32" s="28"/>
@@ -5576,19 +5569,19 @@
       <c r="CF32" s="28"/>
       <c r="CG32" s="28"/>
     </row>
-    <row r="33" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A33" s="32"/>
-      <c r="B33" s="113" t="s">
+      <c r="B33" s="106" t="s">
         <v>52</v>
       </c>
-      <c r="C33" s="114"/>
-      <c r="D33" s="115">
+      <c r="C33" s="107"/>
+      <c r="D33" s="108">
         <v>0</v>
       </c>
-      <c r="E33" s="116">
+      <c r="E33" s="109">
         <v>45976</v>
       </c>
-      <c r="F33" s="116">
+      <c r="F33" s="109">
         <v>45978</v>
       </c>
       <c r="G33" s="11"/>
@@ -5671,15 +5664,15 @@
       <c r="CF33" s="28"/>
       <c r="CG33" s="28"/>
     </row>
-    <row r="34" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A34" s="32"/>
-      <c r="B34" s="119" t="s">
+      <c r="B34" s="112" t="s">
         <v>53</v>
       </c>
-      <c r="C34" s="117"/>
-      <c r="D34" s="118"/>
-      <c r="E34" s="120"/>
-      <c r="F34" s="121"/>
+      <c r="C34" s="110"/>
+      <c r="D34" s="111"/>
+      <c r="E34" s="113"/>
+      <c r="F34" s="114"/>
       <c r="G34" s="11"/>
       <c r="H34" s="11"/>
       <c r="I34" s="28"/>
@@ -5760,7 +5753,7 @@
       <c r="CF34" s="28"/>
       <c r="CG34" s="28"/>
     </row>
-    <row r="35" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A35" s="32"/>
       <c r="B35" s="52" t="s">
         <v>54</v>
@@ -5855,7 +5848,7 @@
       <c r="CF35" s="28"/>
       <c r="CG35" s="28"/>
     </row>
-    <row r="36" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A36" s="32"/>
       <c r="B36" s="52" t="s">
         <v>55</v>
@@ -5944,7 +5937,7 @@
       <c r="CF36" s="28"/>
       <c r="CG36" s="28"/>
     </row>
-    <row r="37" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A37" s="32"/>
       <c r="B37" s="52" t="s">
         <v>56</v>
@@ -6033,15 +6026,15 @@
       <c r="CF37" s="28"/>
       <c r="CG37" s="28"/>
     </row>
-    <row r="38" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A38" s="32"/>
-      <c r="B38" s="122" t="s">
+      <c r="B38" s="115" t="s">
         <v>57</v>
       </c>
-      <c r="C38" s="123"/>
-      <c r="D38" s="124"/>
-      <c r="E38" s="125"/>
-      <c r="F38" s="126"/>
+      <c r="C38" s="116"/>
+      <c r="D38" s="117"/>
+      <c r="E38" s="118"/>
+      <c r="F38" s="119"/>
       <c r="G38" s="11"/>
       <c r="H38" s="11"/>
       <c r="I38" s="28"/>
@@ -6122,19 +6115,19 @@
       <c r="CF38" s="28"/>
       <c r="CG38" s="28"/>
     </row>
-    <row r="39" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A39" s="32"/>
-      <c r="B39" s="127" t="s">
+      <c r="B39" s="120" t="s">
         <v>58</v>
       </c>
-      <c r="C39" s="128"/>
-      <c r="D39" s="129">
+      <c r="C39" s="121"/>
+      <c r="D39" s="122">
         <v>0</v>
       </c>
-      <c r="E39" s="130">
+      <c r="E39" s="123">
         <v>45981</v>
       </c>
-      <c r="F39" s="130">
+      <c r="F39" s="123">
         <v>45982</v>
       </c>
       <c r="G39" s="11"/>
@@ -6217,19 +6210,19 @@
       <c r="CF39" s="28"/>
       <c r="CG39" s="28"/>
     </row>
-    <row r="40" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A40" s="32"/>
-      <c r="B40" s="127" t="s">
+      <c r="B40" s="120" t="s">
         <v>59</v>
       </c>
-      <c r="C40" s="128"/>
-      <c r="D40" s="129">
+      <c r="C40" s="121"/>
+      <c r="D40" s="122">
         <v>0</v>
       </c>
-      <c r="E40" s="130">
+      <c r="E40" s="123">
         <v>45983</v>
       </c>
-      <c r="F40" s="130">
+      <c r="F40" s="123">
         <v>45985</v>
       </c>
       <c r="G40" s="11"/>
@@ -6312,15 +6305,15 @@
       <c r="CF40" s="28"/>
       <c r="CG40" s="28"/>
     </row>
-    <row r="41" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A41" s="32"/>
-      <c r="B41" s="131" t="s">
+      <c r="B41" s="124" t="s">
         <v>60</v>
       </c>
-      <c r="C41" s="132"/>
-      <c r="D41" s="133"/>
-      <c r="E41" s="134"/>
-      <c r="F41" s="135"/>
+      <c r="C41" s="125"/>
+      <c r="D41" s="126"/>
+      <c r="E41" s="127"/>
+      <c r="F41" s="128"/>
       <c r="G41" s="11"/>
       <c r="H41" s="11"/>
       <c r="I41" s="28"/>
@@ -6401,7 +6394,7 @@
       <c r="CF41" s="28"/>
       <c r="CG41" s="28"/>
     </row>
-    <row r="42" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A42" s="32"/>
       <c r="B42" s="51" t="s">
         <v>61</v>
@@ -6496,7 +6489,7 @@
       <c r="CF42" s="28"/>
       <c r="CG42" s="28"/>
     </row>
-    <row r="43" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A43" s="32"/>
       <c r="B43" s="51" t="s">
         <v>62</v>
@@ -6587,15 +6580,15 @@
       <c r="CF43" s="28"/>
       <c r="CG43" s="28"/>
     </row>
-    <row r="44" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A44" s="32"/>
-      <c r="B44" s="103" t="s">
+      <c r="B44" s="96" t="s">
         <v>63</v>
       </c>
-      <c r="C44" s="104"/>
-      <c r="D44" s="105"/>
-      <c r="E44" s="106"/>
-      <c r="F44" s="107"/>
+      <c r="C44" s="97"/>
+      <c r="D44" s="98"/>
+      <c r="E44" s="99"/>
+      <c r="F44" s="100"/>
       <c r="G44" s="11"/>
       <c r="H44" s="11"/>
       <c r="I44" s="28"/>
@@ -6676,7 +6669,7 @@
       <c r="CF44" s="28"/>
       <c r="CG44" s="28"/>
     </row>
-    <row r="45" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A45" s="32"/>
       <c r="B45" s="50" t="s">
         <v>64</v>
@@ -6771,7 +6764,7 @@
       <c r="CF45" s="28"/>
       <c r="CG45" s="28"/>
     </row>
-    <row r="46" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A46" s="32"/>
       <c r="B46" s="50" t="s">
         <v>65</v>
@@ -6866,7 +6859,7 @@
       <c r="CF46" s="28"/>
       <c r="CG46" s="28"/>
     </row>
-    <row r="47" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A47" s="32" t="s">
         <v>12</v>
       </c>
@@ -6958,7 +6951,7 @@
       <c r="CF47" s="28"/>
       <c r="CG47" s="28"/>
     </row>
-    <row r="48" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A48" s="33" t="s">
         <v>13</v>
       </c>
@@ -7052,33 +7045,33 @@
       <c r="CF48" s="30"/>
       <c r="CG48" s="30"/>
     </row>
-    <row r="49" spans="3:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:7" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="G49" s="6"/>
     </row>
-    <row r="50" spans="3:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:7" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C50" s="8"/>
       <c r="F50" s="34"/>
     </row>
-    <row r="51" spans="3:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:7" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C51" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
+    <mergeCell ref="BF4:BL4"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="P4:V4"/>
+    <mergeCell ref="W4:AC4"/>
+    <mergeCell ref="AD4:AJ4"/>
     <mergeCell ref="BM4:BS4"/>
     <mergeCell ref="BT4:BZ4"/>
     <mergeCell ref="CA4:CG4"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
-    <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="P4:V4"/>
-    <mergeCell ref="W4:AC4"/>
-    <mergeCell ref="AD4:AJ4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D48">
     <cfRule type="dataBar" priority="23">
@@ -7095,27 +7088,26 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:BK48 BM5:BR48 BT5:BY48 CA5:CF48">
-    <cfRule type="expression" dxfId="5" priority="42">
+    <cfRule type="expression" dxfId="4" priority="42">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:BK48 BM7:BR48 BT7:BY48 CA7:CF48">
-    <cfRule type="expression" dxfId="4" priority="36">
-      <formula>AND(Fecha_incio&lt;=I$5,ROUNDDOWN((Fecha_final-Fecha_incio+1)*Progresos,0)+Fecha_incio-1&gt;=I$5)</formula>
-    </cfRule>
     <cfRule type="expression" dxfId="3" priority="37" stopIfTrue="1">
       <formula>AND(Fecha_final&gt;=I$5,Fecha_incio&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="I7:CG48">
+    <cfRule type="expression" dxfId="2" priority="36">
+      <formula>AND(Fecha_incio&lt;=I$5,ROUNDDOWN((Fecha_final-Fecha_incio+1)*Progresos,0)+Fecha_incio-1&gt;=I$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="BL5:BL48 BS5:BS48 BZ5:BZ48 CG5:CG48">
-    <cfRule type="expression" dxfId="2" priority="44">
+    <cfRule type="expression" dxfId="1" priority="44">
       <formula>AND(TODAY()&gt;=BL$5,TODAY()&lt;CH$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BL7:BL48 BS7:BS48 BZ7:BZ48 CG7:CG48">
-    <cfRule type="expression" dxfId="1" priority="47">
-      <formula>AND(Fecha_incio&lt;=BL$5,ROUNDDOWN((Fecha_final-Fecha_incio+1)*Progresos,0)+Fecha_incio-1&gt;=BL$5)</formula>
-    </cfRule>
     <cfRule type="expression" dxfId="0" priority="48" stopIfTrue="1">
       <formula>AND(Fecha_final&gt;=BL$5,Fecha_incio&lt;CH$5)</formula>
     </cfRule>
@@ -7166,18 +7158,18 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.45" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.45" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="69" customWidth="1"/>
-    <col min="2" max="2" width="88.28515625" style="69" customWidth="1"/>
-    <col min="3" max="16381" width="10.7109375" style="69" hidden="1"/>
-    <col min="16382" max="16382" width="28.85546875" style="69" hidden="1" customWidth="1"/>
-    <col min="16383" max="16383" width="25.140625" style="69" hidden="1" customWidth="1"/>
-    <col min="16384" max="16384" width="18.28515625" style="69" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="3.265625" style="69" customWidth="1"/>
+    <col min="2" max="2" width="88.265625" style="69" customWidth="1"/>
+    <col min="3" max="16381" width="10.73046875" style="69" hidden="1"/>
+    <col min="16382" max="16382" width="28.86328125" style="69" hidden="1" customWidth="1"/>
+    <col min="16383" max="16383" width="25.1328125" style="69" hidden="1" customWidth="1"/>
+    <col min="16384" max="16384" width="18.265625" style="69" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:2" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:2" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:2" ht="105" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" s="70" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
FIX: Se realizan validaciones de seguridad de la creación de contraseña. Se agregan paginas 404 500 y errores genéricos
</commit_message>
<xml_diff>
--- a/Fase 1/Evidencias Grupales/CartaGantt.xlsx
+++ b/Fase 1/Evidencias Grupales/CartaGantt.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4BFC1A9-638E-475B-9AC7-FAFBE8A28429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FFAF650-9830-4037-B19F-9F1934F2E2E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1534,7 +1534,6 @@
     <xf numFmtId="169" fontId="5" fillId="54" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="171" fontId="15" fillId="42" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1553,6 +1552,7 @@
     <xf numFmtId="170" fontId="9" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="55">
     <cellStyle name="20% - Énfasis1" xfId="31" builtinId="30" customBuiltin="1"/>
@@ -2264,9 +2264,9 @@
   </sheetPr>
   <dimension ref="A1:CG51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D40" sqref="D40"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="CR44" sqref="CR44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2315,148 +2315,148 @@
       <c r="B3" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="133" t="s">
+      <c r="C3" s="132" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="134"/>
-      <c r="E3" s="135">
+      <c r="D3" s="133"/>
+      <c r="E3" s="134">
         <f ca="1">TODAY()</f>
-        <v>45982</v>
-      </c>
-      <c r="F3" s="135"/>
+        <v>45986</v>
+      </c>
+      <c r="F3" s="134"/>
     </row>
     <row r="4" spans="1:85" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="133" t="s">
+      <c r="C4" s="132" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="134"/>
+      <c r="D4" s="133"/>
       <c r="E4" s="7">
-        <v>-6</v>
-      </c>
-      <c r="I4" s="130">
+        <v>-7</v>
+      </c>
+      <c r="I4" s="129">
         <f ca="1">I5</f>
         <v>45929</v>
       </c>
-      <c r="J4" s="131"/>
-      <c r="K4" s="131"/>
-      <c r="L4" s="131"/>
-      <c r="M4" s="131"/>
-      <c r="N4" s="131"/>
-      <c r="O4" s="132"/>
-      <c r="P4" s="130">
+      <c r="J4" s="130"/>
+      <c r="K4" s="130"/>
+      <c r="L4" s="130"/>
+      <c r="M4" s="130"/>
+      <c r="N4" s="130"/>
+      <c r="O4" s="131"/>
+      <c r="P4" s="129">
         <f ca="1">P5</f>
         <v>45936</v>
       </c>
-      <c r="Q4" s="131"/>
-      <c r="R4" s="131"/>
-      <c r="S4" s="131"/>
-      <c r="T4" s="131"/>
-      <c r="U4" s="131"/>
-      <c r="V4" s="132"/>
-      <c r="W4" s="130">
+      <c r="Q4" s="130"/>
+      <c r="R4" s="130"/>
+      <c r="S4" s="130"/>
+      <c r="T4" s="130"/>
+      <c r="U4" s="130"/>
+      <c r="V4" s="131"/>
+      <c r="W4" s="129">
         <f ca="1">W5</f>
         <v>45943</v>
       </c>
-      <c r="X4" s="131"/>
-      <c r="Y4" s="131"/>
-      <c r="Z4" s="131"/>
-      <c r="AA4" s="131"/>
-      <c r="AB4" s="131"/>
-      <c r="AC4" s="132"/>
-      <c r="AD4" s="130">
+      <c r="X4" s="130"/>
+      <c r="Y4" s="130"/>
+      <c r="Z4" s="130"/>
+      <c r="AA4" s="130"/>
+      <c r="AB4" s="130"/>
+      <c r="AC4" s="131"/>
+      <c r="AD4" s="129">
         <f ca="1">AD5</f>
         <v>45950</v>
       </c>
-      <c r="AE4" s="131"/>
-      <c r="AF4" s="131"/>
-      <c r="AG4" s="131"/>
-      <c r="AH4" s="131"/>
-      <c r="AI4" s="131"/>
-      <c r="AJ4" s="132"/>
-      <c r="AK4" s="130">
+      <c r="AE4" s="130"/>
+      <c r="AF4" s="130"/>
+      <c r="AG4" s="130"/>
+      <c r="AH4" s="130"/>
+      <c r="AI4" s="130"/>
+      <c r="AJ4" s="131"/>
+      <c r="AK4" s="129">
         <f ca="1">AK5</f>
         <v>45957</v>
       </c>
-      <c r="AL4" s="131"/>
-      <c r="AM4" s="131"/>
-      <c r="AN4" s="131"/>
-      <c r="AO4" s="131"/>
-      <c r="AP4" s="131"/>
-      <c r="AQ4" s="132"/>
-      <c r="AR4" s="130">
+      <c r="AL4" s="130"/>
+      <c r="AM4" s="130"/>
+      <c r="AN4" s="130"/>
+      <c r="AO4" s="130"/>
+      <c r="AP4" s="130"/>
+      <c r="AQ4" s="131"/>
+      <c r="AR4" s="129">
         <f ca="1">AR5</f>
         <v>45964</v>
       </c>
-      <c r="AS4" s="131"/>
-      <c r="AT4" s="131"/>
-      <c r="AU4" s="131"/>
-      <c r="AV4" s="131"/>
-      <c r="AW4" s="131"/>
-      <c r="AX4" s="132"/>
-      <c r="AY4" s="130">
+      <c r="AS4" s="130"/>
+      <c r="AT4" s="130"/>
+      <c r="AU4" s="130"/>
+      <c r="AV4" s="130"/>
+      <c r="AW4" s="130"/>
+      <c r="AX4" s="131"/>
+      <c r="AY4" s="129">
         <f ca="1">AY5</f>
         <v>45971</v>
       </c>
-      <c r="AZ4" s="131"/>
-      <c r="BA4" s="131"/>
-      <c r="BB4" s="131"/>
-      <c r="BC4" s="131"/>
-      <c r="BD4" s="131"/>
-      <c r="BE4" s="132"/>
-      <c r="BF4" s="130">
+      <c r="AZ4" s="130"/>
+      <c r="BA4" s="130"/>
+      <c r="BB4" s="130"/>
+      <c r="BC4" s="130"/>
+      <c r="BD4" s="130"/>
+      <c r="BE4" s="131"/>
+      <c r="BF4" s="129">
         <f ca="1">BF5</f>
         <v>45978</v>
       </c>
-      <c r="BG4" s="131"/>
-      <c r="BH4" s="131"/>
-      <c r="BI4" s="131"/>
-      <c r="BJ4" s="131"/>
-      <c r="BK4" s="131"/>
-      <c r="BL4" s="132"/>
-      <c r="BM4" s="130">
+      <c r="BG4" s="130"/>
+      <c r="BH4" s="130"/>
+      <c r="BI4" s="130"/>
+      <c r="BJ4" s="130"/>
+      <c r="BK4" s="130"/>
+      <c r="BL4" s="131"/>
+      <c r="BM4" s="129">
         <f ca="1">BM5</f>
         <v>45985</v>
       </c>
-      <c r="BN4" s="131"/>
-      <c r="BO4" s="131"/>
-      <c r="BP4" s="131"/>
-      <c r="BQ4" s="131"/>
-      <c r="BR4" s="131"/>
-      <c r="BS4" s="132"/>
-      <c r="BT4" s="130">
+      <c r="BN4" s="130"/>
+      <c r="BO4" s="130"/>
+      <c r="BP4" s="130"/>
+      <c r="BQ4" s="130"/>
+      <c r="BR4" s="130"/>
+      <c r="BS4" s="131"/>
+      <c r="BT4" s="129">
         <f ca="1">BT5</f>
         <v>45992</v>
       </c>
-      <c r="BU4" s="131"/>
-      <c r="BV4" s="131"/>
-      <c r="BW4" s="131"/>
-      <c r="BX4" s="131"/>
-      <c r="BY4" s="131"/>
-      <c r="BZ4" s="132"/>
-      <c r="CA4" s="130">
+      <c r="BU4" s="130"/>
+      <c r="BV4" s="130"/>
+      <c r="BW4" s="130"/>
+      <c r="BX4" s="130"/>
+      <c r="BY4" s="130"/>
+      <c r="BZ4" s="131"/>
+      <c r="CA4" s="129">
         <f ca="1">CA5</f>
         <v>45999</v>
       </c>
-      <c r="CB4" s="131"/>
-      <c r="CC4" s="131"/>
-      <c r="CD4" s="131"/>
-      <c r="CE4" s="131"/>
-      <c r="CF4" s="131"/>
-      <c r="CG4" s="132"/>
+      <c r="CB4" s="130"/>
+      <c r="CC4" s="130"/>
+      <c r="CD4" s="130"/>
+      <c r="CE4" s="130"/>
+      <c r="CF4" s="130"/>
+      <c r="CG4" s="131"/>
     </row>
     <row r="5" spans="1:85" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="129"/>
-      <c r="C5" s="129"/>
-      <c r="D5" s="129"/>
-      <c r="E5" s="129"/>
-      <c r="F5" s="129"/>
-      <c r="G5" s="129"/>
+      <c r="B5" s="135"/>
+      <c r="C5" s="135"/>
+      <c r="D5" s="135"/>
+      <c r="E5" s="135"/>
+      <c r="F5" s="135"/>
+      <c r="G5" s="135"/>
       <c r="I5" s="74">
         <f ca="1">InicioDelProyecto-WEEKDAY(InicioDelProyecto,1)+2+7*(SemanaParaMostrar-1)</f>
         <v>45929</v>
@@ -5303,7 +5303,7 @@
       </c>
       <c r="C30" s="88"/>
       <c r="D30" s="89">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E30" s="90">
         <v>45972</v>
@@ -5764,7 +5764,7 @@
       </c>
       <c r="C35" s="47"/>
       <c r="D35" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E35" s="65">
         <v>45979</v>
@@ -6126,7 +6126,7 @@
       </c>
       <c r="C39" s="121"/>
       <c r="D39" s="122">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39" s="123">
         <v>45981</v>
@@ -6221,7 +6221,7 @@
       </c>
       <c r="C40" s="121"/>
       <c r="D40" s="122">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40" s="123">
         <v>45983</v>
@@ -7061,12 +7061,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="BM4:BS4"/>
-    <mergeCell ref="BT4:BZ4"/>
-    <mergeCell ref="CA4:CG4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E3:F3"/>
     <mergeCell ref="B5:G5"/>
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
@@ -7076,6 +7070,12 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="BM4:BS4"/>
+    <mergeCell ref="BT4:BZ4"/>
+    <mergeCell ref="CA4:CG4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E3:F3"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D48">
     <cfRule type="dataBar" priority="23">

</xml_diff>